<commit_message>
Fixed Job Upload New Format issues
</commit_message>
<xml_diff>
--- a/e2e-automation/src/test/resources/JobCatalogNewFormat-100 Profiles.xlsx
+++ b/e2e-automation/src/test/resources/JobCatalogNewFormat-100 Profiles.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11219" uniqueCount="3140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11619" uniqueCount="3540">
   <si>
     <t xml:space="preserve">Job Catalog Data Import Template   </t>
   </si>
@@ -9580,6 +9580,1206 @@
   </si>
   <si>
     <t>JOU100-20260122114032</t>
+  </si>
+  <si>
+    <t>Software Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>SE01-20260122165640</t>
+  </si>
+  <si>
+    <t>Data Analyst 20260122165640</t>
+  </si>
+  <si>
+    <t>DA02-20260122165640</t>
+  </si>
+  <si>
+    <t>Product Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>PM03-20260122165640</t>
+  </si>
+  <si>
+    <t>Sales Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>SM04-20260122165640</t>
+  </si>
+  <si>
+    <t>Marketing Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>MS05-20260122165640</t>
+  </si>
+  <si>
+    <t>Human Resources Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>HR06-20260122165640</t>
+  </si>
+  <si>
+    <t>Financial Analyst 20260122165640</t>
+  </si>
+  <si>
+    <t>FA07-20260122165640</t>
+  </si>
+  <si>
+    <t>Accountant 20260122165640</t>
+  </si>
+  <si>
+    <t>AC08-20260122165640</t>
+  </si>
+  <si>
+    <t>Customer Service Representative 20260122165640</t>
+  </si>
+  <si>
+    <t>CS09-20260122165640</t>
+  </si>
+  <si>
+    <t>Operations Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>OM10-20260122165640</t>
+  </si>
+  <si>
+    <t>Quality Assurance Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>QA11-20260122165640</t>
+  </si>
+  <si>
+    <t>DevOps Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>DO12-20260122165640</t>
+  </si>
+  <si>
+    <t>Business Analyst 20260122165640</t>
+  </si>
+  <si>
+    <t>BA13-20260122165640</t>
+  </si>
+  <si>
+    <t>Project Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>PJM14-20260122165640</t>
+  </si>
+  <si>
+    <t>UX Designer 20260122165640</t>
+  </si>
+  <si>
+    <t>UX15-20260122165640</t>
+  </si>
+  <si>
+    <t>Graphic Designer 20260122165640</t>
+  </si>
+  <si>
+    <t>GD16-20260122165640</t>
+  </si>
+  <si>
+    <t>Content Writer 20260122165640</t>
+  </si>
+  <si>
+    <t>CW17-20260122165640</t>
+  </si>
+  <si>
+    <t>Network Administrator 20260122165640</t>
+  </si>
+  <si>
+    <t>NA18-20260122165640</t>
+  </si>
+  <si>
+    <t>Database Administrator 20260122165640</t>
+  </si>
+  <si>
+    <t>DBA19-20260122165640</t>
+  </si>
+  <si>
+    <t>System Administrator 20260122165640</t>
+  </si>
+  <si>
+    <t>SA20-20260122165640</t>
+  </si>
+  <si>
+    <t>Cybersecurity Analyst 20260122165640</t>
+  </si>
+  <si>
+    <t>CA21-20260122165640</t>
+  </si>
+  <si>
+    <t>Legal Counsel 20260122165640</t>
+  </si>
+  <si>
+    <t>LC22-20260122165640</t>
+  </si>
+  <si>
+    <t>Compliance Officer 20260122165640</t>
+  </si>
+  <si>
+    <t>CO23-20260122165640</t>
+  </si>
+  <si>
+    <t>Supply Chain Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>SCM24-20260122165640</t>
+  </si>
+  <si>
+    <t>Logistics Coordinator 20260122165640</t>
+  </si>
+  <si>
+    <t>LOG25-20260122165640</t>
+  </si>
+  <si>
+    <t>Procurement Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>PS26-20260122165640</t>
+  </si>
+  <si>
+    <t>Training Coordinator 20260122165640</t>
+  </si>
+  <si>
+    <t>TC27-20260122165640</t>
+  </si>
+  <si>
+    <t>Recruitment Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>RS28-20260122165640</t>
+  </si>
+  <si>
+    <t>Payroll Administrator 20260122165640</t>
+  </si>
+  <si>
+    <t>PA29-20260122165640</t>
+  </si>
+  <si>
+    <t>Executive Assistant 20260122165640</t>
+  </si>
+  <si>
+    <t>EA30-20260122165640</t>
+  </si>
+  <si>
+    <t>Administrative Assistant 20260122165640</t>
+  </si>
+  <si>
+    <t>AA31-20260122165640</t>
+  </si>
+  <si>
+    <t>Receptionist 20260122165640</t>
+  </si>
+  <si>
+    <t>REC32-20260122165640</t>
+  </si>
+  <si>
+    <t>Sales Executive 20260122165640</t>
+  </si>
+  <si>
+    <t>SEX33-20260122165640</t>
+  </si>
+  <si>
+    <t>Account Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>AM34-20260122165640</t>
+  </si>
+  <si>
+    <t>Business Development Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>BDM35-20260122165640</t>
+  </si>
+  <si>
+    <t>Customer Success Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>CSM36-20260122165640</t>
+  </si>
+  <si>
+    <t>Technical Support Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>TS37-20260122165640</t>
+  </si>
+  <si>
+    <t>Help Desk Technician 20260122165640</t>
+  </si>
+  <si>
+    <t>HD38-20260122165640</t>
+  </si>
+  <si>
+    <t>Marketing Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>MM39-20260122165640</t>
+  </si>
+  <si>
+    <t>Brand Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>BM40-20260122165640</t>
+  </si>
+  <si>
+    <t>Social Media Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>SMM41-20260122165640</t>
+  </si>
+  <si>
+    <t>SEO Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>SEO42-20260122165640</t>
+  </si>
+  <si>
+    <t>Public Relations Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>PR43-20260122165640</t>
+  </si>
+  <si>
+    <t>Communications Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>COM44-20260122165640</t>
+  </si>
+  <si>
+    <t>Research Scientist 20260122165640</t>
+  </si>
+  <si>
+    <t>RES45-20260122165640</t>
+  </si>
+  <si>
+    <t>Laboratory Technician 20260122165640</t>
+  </si>
+  <si>
+    <t>LAB46-20260122165640</t>
+  </si>
+  <si>
+    <t>Clinical Research Coordinator 20260122165640</t>
+  </si>
+  <si>
+    <t>CRC47-20260122165640</t>
+  </si>
+  <si>
+    <t>Pharmacist 20260122165640</t>
+  </si>
+  <si>
+    <t>PH48-20260122165640</t>
+  </si>
+  <si>
+    <t>Nurse 20260122165640</t>
+  </si>
+  <si>
+    <t>NUR49-20260122165640</t>
+  </si>
+  <si>
+    <t>Medical Assistant 20260122165640</t>
+  </si>
+  <si>
+    <t>MA50-20260122165640</t>
+  </si>
+  <si>
+    <t>Physical Therapist 20260122165640</t>
+  </si>
+  <si>
+    <t>PT51-20260122165640</t>
+  </si>
+  <si>
+    <t>Occupational Therapist 20260122165640</t>
+  </si>
+  <si>
+    <t>OT52-20260122165640</t>
+  </si>
+  <si>
+    <t>Radiologic Technologist 20260122165640</t>
+  </si>
+  <si>
+    <t>RT53-20260122165640</t>
+  </si>
+  <si>
+    <t>Construction Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>CM54-20260122165640</t>
+  </si>
+  <si>
+    <t>Civil Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>CE55-20260122165640</t>
+  </si>
+  <si>
+    <t>Mechanical Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>ME56-20260122165640</t>
+  </si>
+  <si>
+    <t>Electrical Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>EE57-20260122165640</t>
+  </si>
+  <si>
+    <t>Manufacturing Engineer 20260122165640</t>
+  </si>
+  <si>
+    <t>MFE58-20260122165640</t>
+  </si>
+  <si>
+    <t>Production Supervisor 20260122165640</t>
+  </si>
+  <si>
+    <t>PRS59-20260122165640</t>
+  </si>
+  <si>
+    <t>Warehouse Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>WM60-20260122165640</t>
+  </si>
+  <si>
+    <t>Inventory Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>INV61-20260122165640</t>
+  </si>
+  <si>
+    <t>Maintenance Technician 20260122165640</t>
+  </si>
+  <si>
+    <t>MT62-20260122165640</t>
+  </si>
+  <si>
+    <t>Facilities Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>FM63-20260122165640</t>
+  </si>
+  <si>
+    <t>Environmental Health and Safety Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>EHS64-20260122165640</t>
+  </si>
+  <si>
+    <t>Security Officer 20260122165640</t>
+  </si>
+  <si>
+    <t>SO65-20260122165640</t>
+  </si>
+  <si>
+    <t>Teacher 20260122165640</t>
+  </si>
+  <si>
+    <t>TEA66-20260122165640</t>
+  </si>
+  <si>
+    <t>Training Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>TRS67-20260122165640</t>
+  </si>
+  <si>
+    <t>Instructional Designer 20260122165640</t>
+  </si>
+  <si>
+    <t>ID68-20260122165640</t>
+  </si>
+  <si>
+    <t>Librarian 20260122165640</t>
+  </si>
+  <si>
+    <t>LIB69-20260122165640</t>
+  </si>
+  <si>
+    <t>Architect 20260122165640</t>
+  </si>
+  <si>
+    <t>ARC70-20260122165640</t>
+  </si>
+  <si>
+    <t>Interior Designer 20260122165640</t>
+  </si>
+  <si>
+    <t>IDE71-20260122165640</t>
+  </si>
+  <si>
+    <t>Real Estate Agent 20260122165640</t>
+  </si>
+  <si>
+    <t>REA72-20260122165640</t>
+  </si>
+  <si>
+    <t>Property Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>PRM73-20260122165640</t>
+  </si>
+  <si>
+    <t>Financial Advisor 20260122165640</t>
+  </si>
+  <si>
+    <t>FIA74-20260122165640</t>
+  </si>
+  <si>
+    <t>Investment Analyst 20260122165640</t>
+  </si>
+  <si>
+    <t>IA75-20260122165640</t>
+  </si>
+  <si>
+    <t>Credit Analyst 20260122165640</t>
+  </si>
+  <si>
+    <t>CRA76-20260122165640</t>
+  </si>
+  <si>
+    <t>Risk Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>RM77-20260122165640</t>
+  </si>
+  <si>
+    <t>Auditor 20260122165640</t>
+  </si>
+  <si>
+    <t>AUD78-20260122165640</t>
+  </si>
+  <si>
+    <t>Tax Specialist 20260122165640</t>
+  </si>
+  <si>
+    <t>TAX79-20260122165640</t>
+  </si>
+  <si>
+    <t>Budget Analyst 20260122165640</t>
+  </si>
+  <si>
+    <t>BUA80-20260122165640</t>
+  </si>
+  <si>
+    <t>Paralegal 20260122165640</t>
+  </si>
+  <si>
+    <t>PAR81-20260122165640</t>
+  </si>
+  <si>
+    <t>Contract Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>CTM82-20260122165640</t>
+  </si>
+  <si>
+    <t>Chef 20260122165640</t>
+  </si>
+  <si>
+    <t>CHF83-20260122165640</t>
+  </si>
+  <si>
+    <t>Restaurant Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>REM84-20260122165640</t>
+  </si>
+  <si>
+    <t>Event Coordinator 20260122165640</t>
+  </si>
+  <si>
+    <t>EVC85-20260122165640</t>
+  </si>
+  <si>
+    <t>Travel Coordinator 20260122165640</t>
+  </si>
+  <si>
+    <t>TRC86-20260122165640</t>
+  </si>
+  <si>
+    <t>Hotel Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>HM87-20260122165640</t>
+  </si>
+  <si>
+    <t>Flight Attendant 20260122165640</t>
+  </si>
+  <si>
+    <t>FA88-20260122165640</t>
+  </si>
+  <si>
+    <t>Pilot 20260122165640</t>
+  </si>
+  <si>
+    <t>PIL89-20260122165640</t>
+  </si>
+  <si>
+    <t>Truck Driver 20260122165640</t>
+  </si>
+  <si>
+    <t>TD90-20260122165640</t>
+  </si>
+  <si>
+    <t>Delivery Driver 20260122165640</t>
+  </si>
+  <si>
+    <t>DD91-20260122165640</t>
+  </si>
+  <si>
+    <t>Retail Store Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>RSM92-20260122165640</t>
+  </si>
+  <si>
+    <t>Sales Associate 20260122165640</t>
+  </si>
+  <si>
+    <t>SAL93-20260122165640</t>
+  </si>
+  <si>
+    <t>Visual Merchandiser 20260122165640</t>
+  </si>
+  <si>
+    <t>VM94-20260122165640</t>
+  </si>
+  <si>
+    <t>Buyer 20260122165640</t>
+  </si>
+  <si>
+    <t>BUY95-20260122165640</t>
+  </si>
+  <si>
+    <t>E-commerce Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>ECM96-20260122165640</t>
+  </si>
+  <si>
+    <t>Digital Marketing Manager 20260122165640</t>
+  </si>
+  <si>
+    <t>DMM97-20260122165640</t>
+  </si>
+  <si>
+    <t>Videographer 20260122165640</t>
+  </si>
+  <si>
+    <t>VID98-20260122165640</t>
+  </si>
+  <si>
+    <t>Photographer 20260122165640</t>
+  </si>
+  <si>
+    <t>PHO99-20260122165640</t>
+  </si>
+  <si>
+    <t>Journalist 20260122165640</t>
+  </si>
+  <si>
+    <t>JOU100-20260122165640</t>
+  </si>
+  <si>
+    <t>Software Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>SE01-20260122170646</t>
+  </si>
+  <si>
+    <t>Data Analyst 20260122170646</t>
+  </si>
+  <si>
+    <t>DA02-20260122170646</t>
+  </si>
+  <si>
+    <t>Product Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>PM03-20260122170646</t>
+  </si>
+  <si>
+    <t>Sales Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>SM04-20260122170646</t>
+  </si>
+  <si>
+    <t>Marketing Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>MS05-20260122170646</t>
+  </si>
+  <si>
+    <t>Human Resources Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>HR06-20260122170646</t>
+  </si>
+  <si>
+    <t>Financial Analyst 20260122170646</t>
+  </si>
+  <si>
+    <t>FA07-20260122170646</t>
+  </si>
+  <si>
+    <t>Accountant 20260122170646</t>
+  </si>
+  <si>
+    <t>AC08-20260122170646</t>
+  </si>
+  <si>
+    <t>Customer Service Representative 20260122170646</t>
+  </si>
+  <si>
+    <t>CS09-20260122170646</t>
+  </si>
+  <si>
+    <t>Operations Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>OM10-20260122170646</t>
+  </si>
+  <si>
+    <t>Quality Assurance Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>QA11-20260122170646</t>
+  </si>
+  <si>
+    <t>DevOps Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>DO12-20260122170646</t>
+  </si>
+  <si>
+    <t>Business Analyst 20260122170646</t>
+  </si>
+  <si>
+    <t>BA13-20260122170646</t>
+  </si>
+  <si>
+    <t>Project Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>PJM14-20260122170646</t>
+  </si>
+  <si>
+    <t>UX Designer 20260122170646</t>
+  </si>
+  <si>
+    <t>UX15-20260122170646</t>
+  </si>
+  <si>
+    <t>Graphic Designer 20260122170646</t>
+  </si>
+  <si>
+    <t>GD16-20260122170646</t>
+  </si>
+  <si>
+    <t>Content Writer 20260122170646</t>
+  </si>
+  <si>
+    <t>CW17-20260122170646</t>
+  </si>
+  <si>
+    <t>Network Administrator 20260122170646</t>
+  </si>
+  <si>
+    <t>NA18-20260122170646</t>
+  </si>
+  <si>
+    <t>Database Administrator 20260122170646</t>
+  </si>
+  <si>
+    <t>DBA19-20260122170646</t>
+  </si>
+  <si>
+    <t>System Administrator 20260122170646</t>
+  </si>
+  <si>
+    <t>SA20-20260122170646</t>
+  </si>
+  <si>
+    <t>Cybersecurity Analyst 20260122170646</t>
+  </si>
+  <si>
+    <t>CA21-20260122170646</t>
+  </si>
+  <si>
+    <t>Legal Counsel 20260122170646</t>
+  </si>
+  <si>
+    <t>LC22-20260122170646</t>
+  </si>
+  <si>
+    <t>Compliance Officer 20260122170646</t>
+  </si>
+  <si>
+    <t>CO23-20260122170646</t>
+  </si>
+  <si>
+    <t>Supply Chain Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>SCM24-20260122170646</t>
+  </si>
+  <si>
+    <t>Logistics Coordinator 20260122170646</t>
+  </si>
+  <si>
+    <t>LOG25-20260122170646</t>
+  </si>
+  <si>
+    <t>Procurement Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>PS26-20260122170646</t>
+  </si>
+  <si>
+    <t>Training Coordinator 20260122170646</t>
+  </si>
+  <si>
+    <t>TC27-20260122170646</t>
+  </si>
+  <si>
+    <t>Recruitment Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>RS28-20260122170646</t>
+  </si>
+  <si>
+    <t>Payroll Administrator 20260122170646</t>
+  </si>
+  <si>
+    <t>PA29-20260122170646</t>
+  </si>
+  <si>
+    <t>Executive Assistant 20260122170646</t>
+  </si>
+  <si>
+    <t>EA30-20260122170646</t>
+  </si>
+  <si>
+    <t>Administrative Assistant 20260122170646</t>
+  </si>
+  <si>
+    <t>AA31-20260122170646</t>
+  </si>
+  <si>
+    <t>Receptionist 20260122170646</t>
+  </si>
+  <si>
+    <t>REC32-20260122170646</t>
+  </si>
+  <si>
+    <t>Sales Executive 20260122170646</t>
+  </si>
+  <si>
+    <t>SEX33-20260122170646</t>
+  </si>
+  <si>
+    <t>Account Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>AM34-20260122170646</t>
+  </si>
+  <si>
+    <t>Business Development Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>BDM35-20260122170646</t>
+  </si>
+  <si>
+    <t>Customer Success Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>CSM36-20260122170646</t>
+  </si>
+  <si>
+    <t>Technical Support Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>TS37-20260122170646</t>
+  </si>
+  <si>
+    <t>Help Desk Technician 20260122170646</t>
+  </si>
+  <si>
+    <t>HD38-20260122170646</t>
+  </si>
+  <si>
+    <t>Marketing Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>MM39-20260122170646</t>
+  </si>
+  <si>
+    <t>Brand Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>BM40-20260122170646</t>
+  </si>
+  <si>
+    <t>Social Media Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>SMM41-20260122170646</t>
+  </si>
+  <si>
+    <t>SEO Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>SEO42-20260122170646</t>
+  </si>
+  <si>
+    <t>Public Relations Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>PR43-20260122170646</t>
+  </si>
+  <si>
+    <t>Communications Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>COM44-20260122170646</t>
+  </si>
+  <si>
+    <t>Research Scientist 20260122170646</t>
+  </si>
+  <si>
+    <t>RES45-20260122170646</t>
+  </si>
+  <si>
+    <t>Laboratory Technician 20260122170646</t>
+  </si>
+  <si>
+    <t>LAB46-20260122170646</t>
+  </si>
+  <si>
+    <t>Clinical Research Coordinator 20260122170646</t>
+  </si>
+  <si>
+    <t>CRC47-20260122170646</t>
+  </si>
+  <si>
+    <t>Pharmacist 20260122170646</t>
+  </si>
+  <si>
+    <t>PH48-20260122170646</t>
+  </si>
+  <si>
+    <t>Nurse 20260122170646</t>
+  </si>
+  <si>
+    <t>NUR49-20260122170646</t>
+  </si>
+  <si>
+    <t>Medical Assistant 20260122170646</t>
+  </si>
+  <si>
+    <t>MA50-20260122170646</t>
+  </si>
+  <si>
+    <t>Physical Therapist 20260122170646</t>
+  </si>
+  <si>
+    <t>PT51-20260122170646</t>
+  </si>
+  <si>
+    <t>Occupational Therapist 20260122170646</t>
+  </si>
+  <si>
+    <t>OT52-20260122170646</t>
+  </si>
+  <si>
+    <t>Radiologic Technologist 20260122170646</t>
+  </si>
+  <si>
+    <t>RT53-20260122170646</t>
+  </si>
+  <si>
+    <t>Construction Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>CM54-20260122170646</t>
+  </si>
+  <si>
+    <t>Civil Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>CE55-20260122170646</t>
+  </si>
+  <si>
+    <t>Mechanical Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>ME56-20260122170646</t>
+  </si>
+  <si>
+    <t>Electrical Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>EE57-20260122170646</t>
+  </si>
+  <si>
+    <t>Manufacturing Engineer 20260122170646</t>
+  </si>
+  <si>
+    <t>MFE58-20260122170646</t>
+  </si>
+  <si>
+    <t>Production Supervisor 20260122170646</t>
+  </si>
+  <si>
+    <t>PRS59-20260122170646</t>
+  </si>
+  <si>
+    <t>Warehouse Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>WM60-20260122170646</t>
+  </si>
+  <si>
+    <t>Inventory Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>INV61-20260122170646</t>
+  </si>
+  <si>
+    <t>Maintenance Technician 20260122170646</t>
+  </si>
+  <si>
+    <t>MT62-20260122170646</t>
+  </si>
+  <si>
+    <t>Facilities Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>FM63-20260122170646</t>
+  </si>
+  <si>
+    <t>Environmental Health and Safety Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>EHS64-20260122170646</t>
+  </si>
+  <si>
+    <t>Security Officer 20260122170646</t>
+  </si>
+  <si>
+    <t>SO65-20260122170646</t>
+  </si>
+  <si>
+    <t>Teacher 20260122170646</t>
+  </si>
+  <si>
+    <t>TEA66-20260122170646</t>
+  </si>
+  <si>
+    <t>Training Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>TRS67-20260122170646</t>
+  </si>
+  <si>
+    <t>Instructional Designer 20260122170646</t>
+  </si>
+  <si>
+    <t>ID68-20260122170646</t>
+  </si>
+  <si>
+    <t>Librarian 20260122170646</t>
+  </si>
+  <si>
+    <t>LIB69-20260122170646</t>
+  </si>
+  <si>
+    <t>Architect 20260122170646</t>
+  </si>
+  <si>
+    <t>ARC70-20260122170646</t>
+  </si>
+  <si>
+    <t>Interior Designer 20260122170646</t>
+  </si>
+  <si>
+    <t>IDE71-20260122170646</t>
+  </si>
+  <si>
+    <t>Real Estate Agent 20260122170646</t>
+  </si>
+  <si>
+    <t>REA72-20260122170646</t>
+  </si>
+  <si>
+    <t>Property Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>PRM73-20260122170646</t>
+  </si>
+  <si>
+    <t>Financial Advisor 20260122170646</t>
+  </si>
+  <si>
+    <t>FIA74-20260122170646</t>
+  </si>
+  <si>
+    <t>Investment Analyst 20260122170646</t>
+  </si>
+  <si>
+    <t>IA75-20260122170646</t>
+  </si>
+  <si>
+    <t>Credit Analyst 20260122170646</t>
+  </si>
+  <si>
+    <t>CRA76-20260122170646</t>
+  </si>
+  <si>
+    <t>Risk Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>RM77-20260122170646</t>
+  </si>
+  <si>
+    <t>Auditor 20260122170646</t>
+  </si>
+  <si>
+    <t>AUD78-20260122170646</t>
+  </si>
+  <si>
+    <t>Tax Specialist 20260122170646</t>
+  </si>
+  <si>
+    <t>TAX79-20260122170646</t>
+  </si>
+  <si>
+    <t>Budget Analyst 20260122170646</t>
+  </si>
+  <si>
+    <t>BUA80-20260122170646</t>
+  </si>
+  <si>
+    <t>Paralegal 20260122170646</t>
+  </si>
+  <si>
+    <t>PAR81-20260122170646</t>
+  </si>
+  <si>
+    <t>Contract Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>CTM82-20260122170646</t>
+  </si>
+  <si>
+    <t>Chef 20260122170646</t>
+  </si>
+  <si>
+    <t>CHF83-20260122170646</t>
+  </si>
+  <si>
+    <t>Restaurant Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>REM84-20260122170646</t>
+  </si>
+  <si>
+    <t>Event Coordinator 20260122170646</t>
+  </si>
+  <si>
+    <t>EVC85-20260122170646</t>
+  </si>
+  <si>
+    <t>Travel Coordinator 20260122170646</t>
+  </si>
+  <si>
+    <t>TRC86-20260122170646</t>
+  </si>
+  <si>
+    <t>Hotel Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>HM87-20260122170646</t>
+  </si>
+  <si>
+    <t>Flight Attendant 20260122170646</t>
+  </si>
+  <si>
+    <t>FA88-20260122170646</t>
+  </si>
+  <si>
+    <t>Pilot 20260122170646</t>
+  </si>
+  <si>
+    <t>PIL89-20260122170646</t>
+  </si>
+  <si>
+    <t>Truck Driver 20260122170646</t>
+  </si>
+  <si>
+    <t>TD90-20260122170646</t>
+  </si>
+  <si>
+    <t>Delivery Driver 20260122170646</t>
+  </si>
+  <si>
+    <t>DD91-20260122170646</t>
+  </si>
+  <si>
+    <t>Retail Store Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>RSM92-20260122170646</t>
+  </si>
+  <si>
+    <t>Sales Associate 20260122170646</t>
+  </si>
+  <si>
+    <t>SAL93-20260122170646</t>
+  </si>
+  <si>
+    <t>Visual Merchandiser 20260122170646</t>
+  </si>
+  <si>
+    <t>VM94-20260122170646</t>
+  </si>
+  <si>
+    <t>Buyer 20260122170646</t>
+  </si>
+  <si>
+    <t>BUY95-20260122170646</t>
+  </si>
+  <si>
+    <t>E-commerce Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>ECM96-20260122170646</t>
+  </si>
+  <si>
+    <t>Digital Marketing Manager 20260122170646</t>
+  </si>
+  <si>
+    <t>DMM97-20260122170646</t>
+  </si>
+  <si>
+    <t>Videographer 20260122170646</t>
+  </si>
+  <si>
+    <t>VID98-20260122170646</t>
+  </si>
+  <si>
+    <t>Photographer 20260122170646</t>
+  </si>
+  <si>
+    <t>PHO99-20260122170646</t>
+  </si>
+  <si>
+    <t>Journalist 20260122170646</t>
+  </si>
+  <si>
+    <t>JOU100-20260122170646</t>
   </si>
 </sst>
 </file>
@@ -10836,10 +12036,10 @@
     </row>
     <row r="7" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>2940</v>
+        <v>3340</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>2941</v>
+        <v>3341</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>134</v>
@@ -10891,10 +12091,10 @@
     </row>
     <row r="8" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>2942</v>
+        <v>3342</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2943</v>
+        <v>3343</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>2375</v>
@@ -10946,10 +12146,10 @@
     </row>
     <row r="9" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>2944</v>
+        <v>3344</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>2945</v>
+        <v>3345</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2380</v>
@@ -10999,10 +12199,10 @@
     </row>
     <row r="10" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>2946</v>
+        <v>3346</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>2947</v>
+        <v>3347</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>220</v>
@@ -11050,10 +12250,10 @@
     </row>
     <row r="11" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>2948</v>
+        <v>3348</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>2949</v>
+        <v>3349</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>187</v>
@@ -11105,10 +12305,10 @@
     </row>
     <row r="12" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>2950</v>
+        <v>3350</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>2951</v>
+        <v>3351</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1106</v>
@@ -11160,10 +12360,10 @@
     </row>
     <row r="13" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>2952</v>
+        <v>3352</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>2953</v>
+        <v>3353</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>306</v>
@@ -11215,10 +12415,10 @@
     </row>
     <row r="14" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>2954</v>
+        <v>3354</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>2955</v>
+        <v>3355</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>306</v>
@@ -11270,10 +12470,10 @@
     </row>
     <row r="15" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>2956</v>
+        <v>3356</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>2957</v>
+        <v>3357</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>130</v>
@@ -11323,10 +12523,10 @@
     </row>
     <row r="16" spans="1:159" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>2958</v>
+        <v>3358</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>2959</v>
+        <v>3359</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>2402</v>
@@ -11378,10 +12578,10 @@
     </row>
     <row r="17" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>2960</v>
+        <v>3360</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>2961</v>
+        <v>3361</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>134</v>
@@ -11427,10 +12627,10 @@
     </row>
     <row r="18" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>2962</v>
+        <v>3362</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>2963</v>
+        <v>3363</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>134</v>
@@ -11482,10 +12682,10 @@
     </row>
     <row r="19" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>2964</v>
+        <v>3364</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>2965</v>
+        <v>3365</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>2375</v>
@@ -11537,10 +12737,10 @@
     </row>
     <row r="20" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>2966</v>
+        <v>3366</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>2967</v>
+        <v>3367</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>2417</v>
@@ -11592,10 +12792,10 @@
     </row>
     <row r="21" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>2968</v>
+        <v>3368</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>2969</v>
+        <v>3369</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>2421</v>
@@ -11647,10 +12847,10 @@
     </row>
     <row r="22" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>2970</v>
+        <v>3370</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>2971</v>
+        <v>3371</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2421</v>
@@ -11698,10 +12898,10 @@
     </row>
     <row r="23" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>2972</v>
+        <v>3372</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>2973</v>
+        <v>3373</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>187</v>
@@ -11753,10 +12953,10 @@
     </row>
     <row r="24" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>2974</v>
+        <v>3374</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>2975</v>
+        <v>3375</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>1124</v>
@@ -11808,10 +13008,10 @@
     </row>
     <row r="25" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>2976</v>
+        <v>3376</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>2977</v>
+        <v>3377</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>1124</v>
@@ -11855,10 +13055,10 @@
     </row>
     <row r="26" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>2978</v>
+        <v>3378</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>2979</v>
+        <v>3379</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>1124</v>
@@ -11910,10 +13110,10 @@
     </row>
     <row r="27" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>2980</v>
+        <v>3380</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>2981</v>
+        <v>3381</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>1124</v>
@@ -11965,10 +13165,10 @@
     </row>
     <row r="28" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>2982</v>
+        <v>3382</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>2983</v>
+        <v>3383</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>176</v>
@@ -12020,10 +13220,10 @@
     </row>
     <row r="29" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>2984</v>
+        <v>3384</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>2985</v>
+        <v>3385</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>2452</v>
@@ -12075,10 +13275,10 @@
     </row>
     <row r="30" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>2986</v>
+        <v>3386</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>2987</v>
+        <v>3387</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>2456</v>
@@ -12128,10 +13328,10 @@
     </row>
     <row r="31" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>2988</v>
+        <v>3388</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>2989</v>
+        <v>3389</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>2460</v>
@@ -12183,10 +13383,10 @@
     </row>
     <row r="32" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>2990</v>
+        <v>3390</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>2991</v>
+        <v>3391</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>2464</v>
@@ -12238,10 +13438,10 @@
     </row>
     <row r="33" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>2992</v>
+        <v>3392</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>2993</v>
+        <v>3393</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>1106</v>
@@ -12293,10 +13493,10 @@
     </row>
     <row r="34" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>2994</v>
+        <v>3394</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>2995</v>
+        <v>3395</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>1106</v>
@@ -12348,10 +13548,10 @@
     </row>
     <row r="35" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>2996</v>
+        <v>3396</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>2997</v>
+        <v>3397</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>1106</v>
@@ -12403,10 +13603,10 @@
     </row>
     <row r="36" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>2998</v>
+        <v>3398</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>2999</v>
+        <v>3399</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>2479</v>
@@ -12458,10 +13658,10 @@
     </row>
     <row r="37" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>3000</v>
+        <v>3400</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>3001</v>
+        <v>3401</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>2479</v>
@@ -12511,10 +13711,10 @@
     </row>
     <row r="38" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>3002</v>
+        <v>3402</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>3003</v>
+        <v>3403</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>2479</v>
@@ -12566,10 +13766,10 @@
     </row>
     <row r="39" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>3004</v>
+        <v>3404</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>3005</v>
+        <v>3405</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>220</v>
@@ -12621,10 +13821,10 @@
     </row>
     <row r="40" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>3006</v>
+        <v>3406</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>3007</v>
+        <v>3407</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>220</v>
@@ -12676,10 +13876,10 @@
     </row>
     <row r="41" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>3008</v>
+        <v>3408</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>3009</v>
+        <v>3409</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>220</v>
@@ -12731,10 +13931,10 @@
     </row>
     <row r="42" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>3010</v>
+        <v>3410</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>3011</v>
+        <v>3411</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>130</v>
@@ -12784,10 +13984,10 @@
     </row>
     <row r="43" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>3012</v>
+        <v>3412</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>3013</v>
+        <v>3413</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>2502</v>
@@ -12839,10 +14039,10 @@
     </row>
     <row r="44" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>3014</v>
+        <v>3414</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>3015</v>
+        <v>3415</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>2502</v>
@@ -12894,10 +14094,10 @@
     </row>
     <row r="45" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>3016</v>
+        <v>3416</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>3017</v>
+        <v>3417</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>187</v>
@@ -12949,10 +14149,10 @@
     </row>
     <row r="46" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>3018</v>
+        <v>3418</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>3019</v>
+        <v>3419</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>187</v>
@@ -13004,10 +14204,10 @@
     </row>
     <row r="47" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>3020</v>
+        <v>3420</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>3021</v>
+        <v>3421</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>187</v>
@@ -13059,10 +14259,10 @@
     </row>
     <row r="48" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>3022</v>
+        <v>3422</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>3023</v>
+        <v>3423</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>187</v>
@@ -13112,10 +14312,10 @@
     </row>
     <row r="49" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>3024</v>
+        <v>3424</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>3025</v>
+        <v>3425</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>30</v>
@@ -13167,10 +14367,10 @@
     </row>
     <row r="50" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>3026</v>
+        <v>3426</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>3027</v>
+        <v>3427</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>30</v>
@@ -13222,10 +14422,10 @@
     </row>
     <row r="51" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>3028</v>
+        <v>3428</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>3029</v>
+        <v>3429</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>422</v>
@@ -13277,10 +14477,10 @@
     </row>
     <row r="52" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>3030</v>
+        <v>3430</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>3031</v>
+        <v>3431</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>422</v>
@@ -13332,10 +14532,10 @@
     </row>
     <row r="53" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>3032</v>
+        <v>3432</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>3033</v>
+        <v>3433</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>422</v>
@@ -13387,10 +14587,10 @@
     </row>
     <row r="54" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>3034</v>
+        <v>3434</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>3035</v>
+        <v>3435</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -13430,10 +14630,10 @@
     </row>
     <row r="55" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>3036</v>
+        <v>3436</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>3037</v>
+        <v>3437</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>2531</v>
@@ -13485,10 +14685,10 @@
     </row>
     <row r="56" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>3038</v>
+        <v>3438</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>3039</v>
+        <v>3439</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>2531</v>
@@ -13540,10 +14740,10 @@
     </row>
     <row r="57" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>3040</v>
+        <v>3440</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>3041</v>
+        <v>3441</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>2531</v>
@@ -13595,10 +14795,10 @@
     </row>
     <row r="58" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>3042</v>
+        <v>3442</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>3043</v>
+        <v>3443</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>2531</v>
@@ -13650,10 +14850,10 @@
     </row>
     <row r="59" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>3044</v>
+        <v>3444</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>3045</v>
+        <v>3445</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5" t="s">
@@ -13701,10 +14901,10 @@
     </row>
     <row r="60" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>3046</v>
+        <v>3446</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>3047</v>
+        <v>3447</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>727</v>
@@ -13756,10 +14956,10 @@
     </row>
     <row r="61" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>3048</v>
+        <v>3448</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>3049</v>
+        <v>3449</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>134</v>
@@ -13811,10 +15011,10 @@
     </row>
     <row r="62" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>3050</v>
+        <v>3450</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>3051</v>
+        <v>3451</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>134</v>
@@ -13866,10 +15066,10 @@
     </row>
     <row r="63" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>3052</v>
+        <v>3452</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>3053</v>
+        <v>3453</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>134</v>
@@ -13917,10 +15117,10 @@
     </row>
     <row r="64" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>3054</v>
+        <v>3454</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>3055</v>
+        <v>3455</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5" t="s">
@@ -13968,10 +15168,10 @@
     </row>
     <row r="65" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>3056</v>
+        <v>3456</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>3057</v>
+        <v>3457</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>204</v>
@@ -14023,10 +15223,10 @@
     </row>
     <row r="66" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>3058</v>
+        <v>3458</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>3059</v>
+        <v>3459</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>2572</v>
@@ -14078,10 +15278,10 @@
     </row>
     <row r="67" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>3060</v>
+        <v>3460</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>3061</v>
+        <v>3461</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>2577</v>
@@ -14133,10 +15333,10 @@
     </row>
     <row r="68" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>3062</v>
+        <v>3462</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>3063</v>
+        <v>3463</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>562</v>
@@ -14188,10 +15388,10 @@
     </row>
     <row r="69" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>3064</v>
+        <v>3464</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>3065</v>
+        <v>3465</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>2586</v>
@@ -14241,10 +15441,10 @@
     </row>
     <row r="70" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>3066</v>
+        <v>3466</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>3067</v>
+        <v>3467</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>2590</v>
@@ -14296,10 +15496,10 @@
     </row>
     <row r="71" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>3068</v>
+        <v>3468</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>3069</v>
+        <v>3469</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>400</v>
@@ -14351,10 +15551,10 @@
     </row>
     <row r="72" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>3070</v>
+        <v>3470</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>3071</v>
+        <v>3471</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>543</v>
@@ -14406,10 +15606,10 @@
     </row>
     <row r="73" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>3072</v>
+        <v>3472</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>3073</v>
+        <v>3473</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5" t="s">
@@ -14459,10 +15659,10 @@
     </row>
     <row r="74" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>3074</v>
+        <v>3474</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>3075</v>
+        <v>3475</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>2603</v>
@@ -14514,10 +15714,10 @@
     </row>
     <row r="75" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>3076</v>
+        <v>3476</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>3077</v>
+        <v>3477</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>543</v>
@@ -14569,10 +15769,10 @@
     </row>
     <row r="76" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>3078</v>
+        <v>3478</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>3079</v>
+        <v>3479</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>2614</v>
@@ -14624,10 +15824,10 @@
     </row>
     <row r="77" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>3080</v>
+        <v>3480</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>3081</v>
+        <v>3481</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>2421</v>
@@ -14679,10 +15879,10 @@
     </row>
     <row r="78" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>3082</v>
+        <v>3482</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>3083</v>
+        <v>3483</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>216</v>
@@ -14734,10 +15934,10 @@
     </row>
     <row r="79" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>3084</v>
+        <v>3484</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>3085</v>
+        <v>3485</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>216</v>
@@ -14789,10 +15989,10 @@
     </row>
     <row r="80" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>3086</v>
+        <v>3486</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>3087</v>
+        <v>3487</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>306</v>
@@ -14844,10 +16044,10 @@
     </row>
     <row r="81" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>3088</v>
+        <v>3488</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>3089</v>
+        <v>3489</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -14893,10 +16093,10 @@
     </row>
     <row r="82" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>3090</v>
+        <v>3490</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>3091</v>
+        <v>3491</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>306</v>
@@ -14948,10 +16148,10 @@
     </row>
     <row r="83" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>3092</v>
+        <v>3492</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>3093</v>
+        <v>3493</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>2637</v>
@@ -15003,10 +16203,10 @@
     </row>
     <row r="84" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>3094</v>
+        <v>3494</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>3095</v>
+        <v>3495</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>2641</v>
@@ -15058,10 +16258,10 @@
     </row>
     <row r="85" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>3096</v>
+        <v>3496</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>3097</v>
+        <v>3497</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>306</v>
@@ -15113,10 +16313,10 @@
     </row>
     <row r="86" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>3098</v>
+        <v>3498</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>3099</v>
+        <v>3499</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>306</v>
@@ -15168,10 +16368,10 @@
     </row>
     <row r="87" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>3100</v>
+        <v>3500</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>3101</v>
+        <v>3501</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>176</v>
@@ -15223,10 +16423,10 @@
     </row>
     <row r="88" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>3102</v>
+        <v>3502</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>3103</v>
+        <v>3503</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>176</v>
@@ -15278,10 +16478,10 @@
     </row>
     <row r="89" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>3104</v>
+        <v>3504</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>3105</v>
+        <v>3505</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>2660</v>
@@ -15333,10 +16533,10 @@
     </row>
     <row r="90" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>3106</v>
+        <v>3506</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>3107</v>
+        <v>3507</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5" t="s">
@@ -15384,10 +16584,10 @@
     </row>
     <row r="91" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>3108</v>
+        <v>3508</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>3109</v>
+        <v>3509</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>2670</v>
@@ -15439,10 +16639,10 @@
     </row>
     <row r="92" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>3110</v>
+        <v>3510</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>3111</v>
+        <v>3511</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>2675</v>
@@ -15494,10 +16694,10 @@
     </row>
     <row r="93" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>3112</v>
+        <v>3512</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>3113</v>
+        <v>3513</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>2662</v>
@@ -15549,10 +16749,10 @@
     </row>
     <row r="94" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>3114</v>
+        <v>3514</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>3115</v>
+        <v>3515</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>2682</v>
@@ -15602,10 +16802,10 @@
     </row>
     <row r="95" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>3116</v>
+        <v>3516</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>3117</v>
+        <v>3517</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>2682</v>
@@ -15657,10 +16857,10 @@
     </row>
     <row r="96" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>3118</v>
+        <v>3518</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>3119</v>
+        <v>3519</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>401</v>
@@ -15712,10 +16912,10 @@
     </row>
     <row r="97" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>3120</v>
+        <v>3520</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>3121</v>
+        <v>3521</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>401</v>
@@ -15767,10 +16967,10 @@
     </row>
     <row r="98" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>3122</v>
+        <v>3522</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>3123</v>
+        <v>3523</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>66</v>
@@ -15822,10 +17022,10 @@
     </row>
     <row r="99" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>3124</v>
+        <v>3524</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>3125</v>
+        <v>3525</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>66</v>
@@ -15877,10 +17077,10 @@
     </row>
     <row r="100" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>3126</v>
+        <v>3526</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>3127</v>
+        <v>3527</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>66</v>
@@ -15932,10 +17132,10 @@
     </row>
     <row r="101" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>3128</v>
+        <v>3528</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>3129</v>
+        <v>3529</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>66</v>
@@ -15981,10 +17181,10 @@
     </row>
     <row r="102" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>3130</v>
+        <v>3530</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>3131</v>
+        <v>3531</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>2708</v>
@@ -16036,10 +17236,10 @@
     </row>
     <row r="103" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>3132</v>
+        <v>3532</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>3133</v>
+        <v>3533</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>187</v>
@@ -16091,10 +17291,10 @@
     </row>
     <row r="104" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>3134</v>
+        <v>3534</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>3135</v>
+        <v>3535</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>43</v>
@@ -16146,10 +17346,10 @@
     </row>
     <row r="105" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>3136</v>
+        <v>3536</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>3137</v>
+        <v>3537</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>43</v>
@@ -16199,10 +17399,10 @@
     </row>
     <row r="106" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>3138</v>
+        <v>3538</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>3139</v>
+        <v>3539</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>43</v>

</xml_diff>